<commit_message>
many changes made final changes from my side
</commit_message>
<xml_diff>
--- a/Project/testdata/data.xlsx
+++ b/Project/testdata/data.xlsx
@@ -6,6 +6,7 @@
     <sheet name="SearchBarData" sheetId="1" r:id="rId1"/>
     <sheet name="AssertData" sheetId="2" r:id="rId2"/>
     <sheet name="CheckBoxData" sheetId="3" r:id="rId3"/>
+    <sheet name="InputData" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -406,7 +407,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Adidas</v>
+        <v>ADIDAS</v>
       </c>
     </row>
   </sheetData>
@@ -418,7 +419,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,7 +431,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>adidas</v>
+        <v>ADIDAS</v>
       </c>
     </row>
     <row r="3">
@@ -458,9 +459,49 @@
         <v>Running</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>BADMINTON RACKETS</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>YONEX ARCSABER 2 FEEL</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>CART</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Product added to cart</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>YONEX</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>ZIPCODE</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>shoes</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>required</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A15"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -502,4 +543,23 @@
     <ignoredError numberStoredAsText="1" sqref="A1:A5"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>641001</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test case 9 and 10 done and dusted
</commit_message>
<xml_diff>
--- a/Project/testdata/data.xlsx
+++ b/Project/testdata/data.xlsx
@@ -6,6 +6,9 @@
     <sheet name="SearchBarData" sheetId="1" r:id="rId1"/>
     <sheet name="AssertData" sheetId="2" r:id="rId2"/>
     <sheet name="CheckBoxData" sheetId="3" r:id="rId3"/>
+    <sheet name="PageURLS" sheetId="4" r:id="rId4"/>
+    <sheet name="DataToBeSent" sheetId="5" r:id="rId5"/>
+    <sheet name="AssertContainsData" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -406,7 +409,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Adidas</v>
+        <v>ADIDAS</v>
       </c>
     </row>
   </sheetData>
@@ -418,7 +421,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -427,6 +430,9 @@
       <c r="A1" t="str">
         <v>Search</v>
       </c>
+      <c r="D1" t="str">
+        <v/>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -460,7 +466,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -502,4 +508,128 @@
     <ignoredError numberStoredAsText="1" sqref="A1:A5"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>https://sportsjam.in/</v>
+      </c>
+      <c r="C1" t="str">
+        <v>https://sportsjam.in/sports/cricket-equipment-store-online-india/cricket-shoes-shop-online-india</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>https://sportsjam.in/shopbrand</v>
+      </c>
+      <c r="C2" t="str">
+        <v>https://sportsjam.in/</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>https://sportsjam.in/shopbrand/puma</v>
+      </c>
+      <c r="C3" t="str">
+        <v>https://sportsjam.in/badminton-shoes-online-india</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>https://sportsjam.in/ox_quickview/catalog_product/view/id/30663/</v>
+      </c>
+      <c r="C4" t="str">
+        <v>https://sportsjam.in/sports/basketball-gear-online-india/basketball-shoes-online-india</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="str">
+        <v>https://sportsjam.in/sports/buy-sports-football/football-shoes-online-india</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="str">
+        <v>https://sportsjam.in/buy-running/buy-running-shoes-online-india</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="str">
+        <v>https://sportsjam.in/indoor-court-squash-shoes-online-india</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Puma</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>test134@gmail.com</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>test140@ga</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A3"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Puma</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>accessories</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>you must login or register to add items to your wishlist.</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>THE ACCOUNT SIGN-IN WAS INCORRECT OR YOUR ACCOUNT IS DISABLED TEMPORARILY. PLEASE WAIT AND TRY AGAIN LATER.</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A4"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
All changes Made and bestPractices Done and testCases are done
</commit_message>
<xml_diff>
--- a/Project/testdata/data.xlsx
+++ b/Project/testdata/data.xlsx
@@ -11,7 +11,8 @@
     <sheet name="DataToBeSent" sheetId="6" r:id="rId6"/>
     <sheet name="AssertContainsData" sheetId="7" r:id="rId7"/>
     <sheet name="LoginSheet" sheetId="8" r:id="rId8"/>
-    <sheet name="sheet10" sheetId="9" r:id="rId9"/>
+    <sheet name="InputData" sheetId="9" r:id="rId9"/>
+    <sheet name="sheet11" sheetId="10" r:id="rId10"/>
   </sheets>
 </workbook>
 </file>
@@ -422,9 +423,22 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -436,7 +450,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>adidas</v>
+        <v>ADIDAS</v>
       </c>
     </row>
     <row r="3">
@@ -464,9 +478,49 @@
         <v>Running</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>BADMINTON RACKETS</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>YONEX ARCSABER 2 FEEL</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>CART</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>ADDED TO CART</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>ADDED YONEX</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>ENTER ZIPCODE</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>shoes</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>required</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A15"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -512,22 +566,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Gagandeep</v>
+        <v>wertyuilkjgfdsxcv</v>
       </c>
       <c r="B1" t="str">
-        <v>gagande4@gmail.com</v>
+        <v>fghjfds4@gmail.com</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Kanta</v>
+        <v>dsfdfhgf</v>
       </c>
       <c r="B2" t="str">
         <v>Qwertasdf@#$7654</v>
@@ -538,9 +592,14 @@
         <v>Qwertasdf@#$7654</v>
       </c>
     </row>
+    <row r="7">
+      <c r="D7" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -744,7 +803,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>641001</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>

</xml_diff>